<commit_message>
Net Present Value Calculation
Set up net present value function and formated numeric values to round to 2 decimal places
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Variable</t>
   </si>
@@ -96,6 +96,21 @@
   </si>
   <si>
     <t>https://www.bls.gov/oes/current/oes291022.htm</t>
+  </si>
+  <si>
+    <t>https://nces.ed.gov/programs/digest/d16/tables/dt16_330.40.asp?current=yes</t>
+  </si>
+  <si>
+    <t>https://studentaid.ed.gov/sa/types/loans/interest-rates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.treasury.gov/resource-center/data-chart-center/interest-rates/Pages/TextView.aspx?data=yield </t>
+  </si>
+  <si>
+    <t>https://studentaid.ed.gov/sa/repay-loans/understand/plans</t>
+  </si>
+  <si>
+    <t>https://www.medscape.com/features/slideshow/public/residents-salary-and-debt-report-2016#page=2</t>
   </si>
 </sst>
 </file>
@@ -433,9 +448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -444,7 +457,7 @@
     <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" style="5" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="68.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="72.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
@@ -479,15 +492,21 @@
         <v>10</v>
       </c>
       <c r="D2" s="6"/>
+      <c r="F2" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3" s="2">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3" s="6"/>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -504,13 +523,22 @@
       <c r="C5">
         <v>5</v>
       </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="4">
-        <v>55400</v>
+        <v>56500</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2016</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -605,6 +633,9 @@
       <c r="C12" s="3">
         <v>3.2000000000000001E-2</v>
       </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
@@ -616,6 +647,9 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="3"/>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -627,6 +661,9 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="3"/>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -636,8 +673,20 @@
         <v>3.1600000000000003E-2</v>
       </c>
       <c r="D15" s="6"/>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F13" r:id="rId1"/>
+    <hyperlink ref="F14" r:id="rId2"/>
+    <hyperlink ref="F15" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
+    <hyperlink ref="F6" r:id="rId6" location="page=2"/>
+    <hyperlink ref="F5" r:id="rId7" location="page=2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>